<commit_message>
update xlsx and add print
</commit_message>
<xml_diff>
--- a/resources/analysis_of_algorithms.xlsx
+++ b/resources/analysis_of_algorithms.xlsx
@@ -8,34 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/murillo/development/project/git/private/estudos/searching-sorting-algorithms/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84427AB1-7234-BA45-AE4B-96AFB1684035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2819C2E-9947-204C-B89C-C043E64D2313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="37700" windowHeight="21140" activeTab="4" xr2:uid="{947E0903-3BAA-4B47-9B05-889BB2447F05}"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="37700" windowHeight="21140" activeTab="2" xr2:uid="{947E0903-3BAA-4B47-9B05-889BB2447F05}"/>
   </bookViews>
   <sheets>
     <sheet name="Illustration-Demonstration" sheetId="7" r:id="rId1"/>
     <sheet name="Search Lowest Value - Linear" sheetId="1" r:id="rId2"/>
-    <sheet name="SelectionSort - Quadratic" sheetId="3" r:id="rId3"/>
-    <sheet name="InsertionSort - Quadratic" sheetId="6" r:id="rId4"/>
-    <sheet name="Linear x Quadratic" sheetId="5" r:id="rId5"/>
+    <sheet name="Binary Search" sheetId="8" r:id="rId3"/>
+    <sheet name="SelectionSort - Quadratic" sheetId="3" r:id="rId4"/>
+    <sheet name="InsertionSort - Quadratic" sheetId="6" r:id="rId5"/>
+    <sheet name="Linear x Quadratic" sheetId="5" r:id="rId6"/>
+    <sheet name="MergeSort - QuickSort" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Element Number</t>
   </si>
@@ -70,19 +66,10 @@
     <t>In algorithm analysis we are always concerned with power, as it will make all the difference in the comparison.</t>
   </si>
   <si>
-    <t>2*n^2</t>
-  </si>
-  <si>
-    <t>n^2</t>
-  </si>
-  <si>
     <t>TIME IN SECONDS (8000 Operations)</t>
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>N^2</t>
   </si>
   <si>
     <t>In this algorithm, we execute a 'for' that sweeps N elements, where we can make N elements to the left too, however, we have a call to another algorithm (search for the lowest value), where it can also have the same complexity already analyzed. So, in this case, we have N elements increased to 2 and we can have twice that.</t>
@@ -95,12 +82,6 @@
   </si>
   <si>
     <t>O n</t>
-  </si>
-  <si>
-    <t>n^3</t>
-  </si>
-  <si>
-    <t>2^n</t>
   </si>
   <si>
     <t>Constant</t>
@@ -125,6 +106,39 @@
   </si>
   <si>
     <t>O 2ⁿ</t>
+  </si>
+  <si>
+    <t>MergeSort and QuickSort are of equal size, what should be analyzed are the smallest details, but analysts say that on average QuickSort is faster.</t>
+  </si>
+  <si>
+    <t>Remembering that QuickSorte uses Pivo for its algorithm.</t>
+  </si>
+  <si>
+    <t>MergeSort and QuickSort</t>
+  </si>
+  <si>
+    <t>n*O (log₂ n)</t>
+  </si>
+  <si>
+    <t>log₂ n</t>
+  </si>
+  <si>
+    <t>2*n²</t>
+  </si>
+  <si>
+    <t>n²</t>
+  </si>
+  <si>
+    <t>N²</t>
+  </si>
+  <si>
+    <t>n³</t>
+  </si>
+  <si>
+    <t>2ⁿ</t>
+  </si>
+  <si>
+    <t>Logarithm</t>
   </si>
 </sst>
 </file>
@@ -162,7 +176,7 @@
       <name val="Fira Code"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +225,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -239,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -273,6 +293,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,7 +572,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n^2</c:v>
+                  <c:v>n²</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -636,7 +659,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n^3</c:v>
+                  <c:v>n³</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -723,7 +746,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2^n</c:v>
+                  <c:v>2ⁿ</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -798,6 +821,93 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-2B26-4143-83FB-1FFC81018501}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Illustration-Demonstration'!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n*O (log₂ n)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Illustration-Demonstration'!$A$6:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Illustration-Demonstration'!$G$6:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3B42-5E47-9701-EA00E095CC2D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1851,7 +1961,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>SelectionSort - Quadratic</a:t>
+              <a:t>Binary Search</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1896,11 +2006,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SelectionSort - Quadratic'!$B$6</c:f>
+              <c:f>'Binary Search'!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n^2</c:v>
+                  <c:v>n</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1931,7 +2041,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SelectionSort - Quadratic'!$A$7:$A$20</c:f>
+              <c:f>'Binary Search'!$A$7:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1982,7 +2092,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SelectionSort - Quadratic'!$B$7:$B$20</c:f>
+              <c:f>'Binary Search'!$B$7:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1990,43 +2100,43 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>256</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1024</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>4096</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>65536</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>262144</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1048576</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4194304</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16777216</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>67108864</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2034,7 +2144,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B00D-754F-A261-AE96BBE17AAE}"/>
+              <c16:uniqueId val="{00000000-DB78-EC4F-9E11-6DC5C4333CAC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2043,11 +2153,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SelectionSort - Quadratic'!$C$6</c:f>
+              <c:f>'Binary Search'!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2*n^2</c:v>
+                  <c:v>log₂ n</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2078,7 +2188,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'SelectionSort - Quadratic'!$A$7:$A$20</c:f>
+              <c:f>'Binary Search'!$A$7:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2129,51 +2239,51 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'SelectionSort - Quadratic'!$C$7:$C$20</c:f>
+              <c:f>'Binary Search'!$C$7:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32768</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>131072</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>524288</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2097152</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8388608</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33554432</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>134217728</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2181,7 +2291,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B00D-754F-A261-AE96BBE17AAE}"/>
+              <c16:uniqueId val="{00000001-DB78-EC4F-9E11-6DC5C4333CAC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2543,7 +2653,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>InsertionSort - Quadratic</a:t>
+              <a:t>SelectionSort - Quadratic</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2588,11 +2698,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'InsertionSort - Quadratic'!$B$6</c:f>
+              <c:f>'SelectionSort - Quadratic'!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n^2</c:v>
+                  <c:v>n²</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2623,7 +2733,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'InsertionSort - Quadratic'!$A$7:$A$20</c:f>
+              <c:f>'SelectionSort - Quadratic'!$A$7:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2674,7 +2784,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'InsertionSort - Quadratic'!$B$7:$B$20</c:f>
+              <c:f>'SelectionSort - Quadratic'!$B$7:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2726,7 +2836,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C269-E644-AA1A-DFA124B39C12}"/>
+              <c16:uniqueId val="{00000000-B00D-754F-A261-AE96BBE17AAE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2735,11 +2845,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'InsertionSort - Quadratic'!$C$6</c:f>
+              <c:f>'SelectionSort - Quadratic'!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2*n^2</c:v>
+                  <c:v>2*n²</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2770,7 +2880,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'InsertionSort - Quadratic'!$A$7:$A$20</c:f>
+              <c:f>'SelectionSort - Quadratic'!$A$7:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2821,7 +2931,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'InsertionSort - Quadratic'!$C$7:$C$20</c:f>
+              <c:f>'SelectionSort - Quadratic'!$C$7:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2873,7 +2983,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C269-E644-AA1A-DFA124B39C12}"/>
+              <c16:uniqueId val="{00000001-B00D-754F-A261-AE96BBE17AAE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3232,6 +3342,698 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>InsertionSort - Quadratic</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'InsertionSort - Quadratic'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n²</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'InsertionSort - Quadratic'!$A$7:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'InsertionSort - Quadratic'!$B$7:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>67108864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C269-E644-AA1A-DFA124B39C12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'InsertionSort - Quadratic'!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2*n²</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'InsertionSort - Quadratic'!$A$7:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'InsertionSort - Quadratic'!$C$7:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>134217728</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C269-E644-AA1A-DFA124B39C12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1351367231"/>
+        <c:axId val="1342358879"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1351367231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1342358879"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1342358879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Operations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1351367231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Linear x Quadratic</a:t>
             </a:r>
@@ -3576,7 +4378,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n^2</c:v>
+                  <c:v>n²</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3723,7 +4525,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2*n^2</c:v>
+                  <c:v>2*n²</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4182,7 +4984,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4457,7 +5259,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n^2</c:v>
+                  <c:v>n²</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4550,7 +5352,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2*n^2</c:v>
+                  <c:v>2*n²</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4955,6 +5757,738 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>MergeSort - QuickSort (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Logarithm</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MergeSort - QuickSort'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n*O (log₂ n)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MergeSort - QuickSort'!$A$7:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MergeSort - QuickSort'!$B$7:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4608</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22528</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49152</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>106496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B549-2942-A6F8-61A2EFE9B4C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MergeSort - QuickSort'!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n*O (log₂ n)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MergeSort - QuickSort'!$A$7:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MergeSort - QuickSort'!$C$7:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4608</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22528</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49152</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>106496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B549-2942-A6F8-61A2EFE9B4C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1351367231"/>
+        <c:axId val="1342358879"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1351367231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1342358879"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1342358879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Operations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1351367231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5195,6 +6729,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8291,20 +9905,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>77542</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>113829</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>18144</xdr:rowOff>
+      <xdr:rowOff>45358</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>294777</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>175054</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>331064</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>2696</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8380,6 +11026,49 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
+      <xdr:colOff>108142</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>244784</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>487948</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>187156</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D927F34A-4A1C-FB49-8BF6-D81CE26463D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>148248</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>251470</xdr:rowOff>
@@ -8418,7 +11107,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8461,7 +11150,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8532,6 +11221,49 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>128193</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>251470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>193842</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{313D4240-DE58-DA43-A5B9-EC84CCAE2FD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8840,19 +11572,23 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -8864,36 +11600,42 @@
     <row r="2" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -8907,13 +11649,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -8938,6 +11683,10 @@
       <c r="F6" s="8">
         <f>POWER(2,A6)</f>
         <v>2</v>
+      </c>
+      <c r="G6" s="8">
+        <f>LOG(A6,2)*A6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -8964,6 +11713,10 @@
         <f t="shared" ref="F7:F19" si="2">POWER(2,A7)</f>
         <v>4</v>
       </c>
+      <c r="G7" s="8">
+        <f t="shared" ref="G7:G19" si="3">LOG(A7,2)*A7</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
@@ -8982,12 +11735,16 @@
         <v>16</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" ref="E8:E19" si="3">POWER(A8,3)</f>
+        <f t="shared" ref="E8:G19" si="4">POWER(A8,3)</f>
         <v>64</v>
       </c>
       <c r="F8" s="8">
         <f t="shared" si="2"/>
         <v>16</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -9007,17 +11764,21 @@
         <v>64</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>512</v>
       </c>
       <c r="F9" s="8">
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
+      <c r="G9" s="8">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <f t="shared" ref="A10:A19" si="4">A9*2</f>
+        <f t="shared" ref="A10:A19" si="5">A9*2</f>
         <v>16</v>
       </c>
       <c r="B10" s="4">
@@ -9032,17 +11793,21 @@
         <v>256</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4096</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
         <v>65536</v>
       </c>
+      <c r="G10" s="14">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="B11" s="4">
@@ -9057,17 +11822,21 @@
         <v>1024</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32768</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
         <v>4294967296</v>
       </c>
+      <c r="G11" s="14">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64</v>
       </c>
       <c r="B12" s="4">
@@ -9082,17 +11851,21 @@
         <v>4096</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>262144</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
         <v>1.8446744073709552E+19</v>
       </c>
+      <c r="G12" s="14">
+        <f t="shared" si="3"/>
+        <v>384</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>128</v>
       </c>
       <c r="B13" s="4">
@@ -9107,17 +11880,21 @@
         <v>16384</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2097152</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="2"/>
         <v>3.4028236692093846E+38</v>
       </c>
+      <c r="G13" s="14">
+        <f t="shared" si="3"/>
+        <v>896</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>256</v>
       </c>
       <c r="B14" s="4">
@@ -9132,17 +11909,21 @@
         <v>65536</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16777216</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="2"/>
         <v>1.157920892373162E+77</v>
       </c>
+      <c r="G14" s="14">
+        <f t="shared" si="3"/>
+        <v>2048</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>512</v>
       </c>
       <c r="B15" s="4">
@@ -9157,17 +11938,21 @@
         <v>262144</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>134217728</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="2"/>
         <v>1.3407807929942597E+154</v>
       </c>
+      <c r="G15" s="14">
+        <f t="shared" si="3"/>
+        <v>4608</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1024</v>
       </c>
       <c r="B16" s="9">
@@ -9182,17 +11967,21 @@
         <v>1048576</v>
       </c>
       <c r="E16" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1073741824</v>
       </c>
       <c r="F16" s="9" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
+      <c r="G16" s="14">
+        <f t="shared" si="3"/>
+        <v>10240</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2048</v>
       </c>
       <c r="B17" s="9">
@@ -9207,17 +11996,21 @@
         <v>4194304</v>
       </c>
       <c r="E17" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8589934592</v>
       </c>
       <c r="F17" s="9" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
+      <c r="G17" s="14">
+        <f t="shared" si="3"/>
+        <v>22528</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4096</v>
       </c>
       <c r="B18" s="9">
@@ -9232,17 +12025,21 @@
         <v>16777216</v>
       </c>
       <c r="E18" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68719476736</v>
       </c>
       <c r="F18" s="9" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
+      <c r="G18" s="14">
+        <f t="shared" si="3"/>
+        <v>49152</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8192</v>
       </c>
       <c r="B19" s="9">
@@ -9257,12 +12054,16 @@
         <v>67108864</v>
       </c>
       <c r="E19" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>549755813888</v>
       </c>
       <c r="F19" s="9" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
+      </c>
+      <c r="G19" s="14">
+        <f t="shared" si="3"/>
+        <v>106496</v>
       </c>
     </row>
   </sheetData>
@@ -9524,11 +12325,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B93DAC-644C-E247-983E-BA135F125625}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869651EC-967B-C04A-840E-2BD30F4B1AAF}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9549,16 +12350,8 @@
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -9566,10 +12359,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -9577,96 +12370,92 @@
         <v>1</v>
       </c>
       <c r="B7" s="4">
-        <f>A7*A7</f>
+        <f>A7</f>
         <v>1</v>
       </c>
       <c r="C7" s="4">
-        <f>B7*2</f>
-        <v>2</v>
+        <f>LOG(A7,2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <f>A7*2</f>
         <v>2</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" ref="B8:B20" si="0">A8*A8</f>
-        <v>4</v>
+        <f>A8</f>
+        <v>2</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" ref="C8:C20" si="1">B8*2</f>
-        <v>8</v>
+        <f t="shared" ref="C8:C20" si="0">LOG(A8,2)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <f>A8*2</f>
         <v>4</v>
       </c>
       <c r="B9" s="4">
+        <f t="shared" ref="B9:B20" si="1">A9</f>
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <f>A9*2</f>
         <v>8</v>
       </c>
       <c r="B10" s="4">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>128</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <f t="shared" ref="A11:A20" si="2">A10*2</f>
         <v>16</v>
       </c>
       <c r="B11" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>256</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>512</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <f t="shared" si="2"/>
+        <f>2*A11</f>
         <v>32</v>
       </c>
       <c r="B12" s="4">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>1024</v>
-      </c>
-      <c r="C12" s="4">
-        <f t="shared" si="1"/>
-        <v>2048</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A13:A20" si="2">2*A12</f>
         <v>64</v>
       </c>
       <c r="B13" s="4">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>4096</v>
-      </c>
-      <c r="C13" s="4">
-        <f t="shared" si="1"/>
-        <v>8192</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -9675,12 +12464,12 @@
         <v>128</v>
       </c>
       <c r="B14" s="4">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>16384</v>
-      </c>
-      <c r="C14" s="4">
-        <f t="shared" si="1"/>
-        <v>32768</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -9689,12 +12478,12 @@
         <v>256</v>
       </c>
       <c r="B15" s="4">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="C15" s="4">
         <f t="shared" si="0"/>
-        <v>65536</v>
-      </c>
-      <c r="C15" s="4">
-        <f t="shared" si="1"/>
-        <v>131072</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -9703,12 +12492,12 @@
         <v>512</v>
       </c>
       <c r="B16" s="4">
+        <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
+      <c r="C16" s="4">
         <f t="shared" si="0"/>
-        <v>262144</v>
-      </c>
-      <c r="C16" s="4">
-        <f t="shared" si="1"/>
-        <v>524288</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -9717,12 +12506,12 @@
         <v>1024</v>
       </c>
       <c r="B17" s="4">
+        <f t="shared" si="1"/>
+        <v>1024</v>
+      </c>
+      <c r="C17" s="4">
         <f t="shared" si="0"/>
-        <v>1048576</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" si="1"/>
-        <v>2097152</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -9731,12 +12520,12 @@
         <v>2048</v>
       </c>
       <c r="B18" s="4">
+        <f t="shared" si="1"/>
+        <v>2048</v>
+      </c>
+      <c r="C18" s="4">
         <f t="shared" si="0"/>
-        <v>4194304</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="1"/>
-        <v>8388608</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -9745,12 +12534,12 @@
         <v>4096</v>
       </c>
       <c r="B19" s="4">
+        <f t="shared" si="1"/>
+        <v>4096</v>
+      </c>
+      <c r="C19" s="4">
         <f t="shared" si="0"/>
-        <v>16777216</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="1"/>
-        <v>33554432</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -9759,12 +12548,12 @@
         <v>8192</v>
       </c>
       <c r="B20" s="4">
+        <f t="shared" si="1"/>
+        <v>8192</v>
+      </c>
+      <c r="C20" s="4">
         <f t="shared" si="0"/>
-        <v>67108864</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="1"/>
-        <v>134217728</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -9777,11 +12566,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6849EDD3-74E9-FF46-88EC-C3FB561B1C2B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B93DAC-644C-E247-983E-BA135F125625}">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9804,7 +12593,7 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9819,10 +12608,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -10030,11 +12819,264 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6849EDD3-74E9-FF46-88EC-C3FB561B1C2B}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <f>A7*A7</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <f>B7*2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <f>A7*2</f>
+        <v>2</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" ref="B8:B20" si="0">A8*A8</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" ref="C8:C20" si="1">B8*2</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <f>A8*2</f>
+        <v>4</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <f>A9*2</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <f t="shared" ref="A11:A20" si="2">A10*2</f>
+        <v>16</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="1"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>4096</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="1"/>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>16384</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="1"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>65536</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="1"/>
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <f t="shared" si="2"/>
+        <v>512</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="1"/>
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <f t="shared" si="2"/>
+        <v>1024</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>1048576</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="1"/>
+        <v>2097152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <f t="shared" si="2"/>
+        <v>2048</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>4194304</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="1"/>
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <f t="shared" si="2"/>
+        <v>4096</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="0"/>
+        <v>16777216</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="1"/>
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <f t="shared" si="2"/>
+        <v>8192</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="0"/>
+        <v>67108864</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="1"/>
+        <v>134217728</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F65158-399C-A343-AD2B-B9814A7285B0}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10080,16 +13122,16 @@
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -10513,7 +13555,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F21" s="13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G21" s="13"/>
     </row>
@@ -10535,10 +13577,10 @@
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -10721,4 +13763,256 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3702F7DE-5470-4F43-AE3E-BA5F31FF4180}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <f>LOG(A7,2)*A7</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <f>LOG(A7,2)*A7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <f>A7*2</f>
+        <v>2</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" ref="B8:B20" si="0">LOG(A8,2)*A8</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" ref="C8:C20" si="1">LOG(A8,2)*A8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <f>A8*2</f>
+        <v>4</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <f>A9*2</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <f t="shared" ref="A11:A20" si="2">A10*2</f>
+        <v>16</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>384</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>896</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="1"/>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="1"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <f t="shared" si="2"/>
+        <v>512</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>4608</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="1"/>
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <f t="shared" si="2"/>
+        <v>1024</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>10240</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="1"/>
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <f t="shared" si="2"/>
+        <v>2048</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>22528</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="1"/>
+        <v>22528</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <f t="shared" si="2"/>
+        <v>4096</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="0"/>
+        <v>49152</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="1"/>
+        <v>49152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <f t="shared" si="2"/>
+        <v>8192</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="0"/>
+        <v>106496</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="1"/>
+        <v>106496</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update prints and contents
</commit_message>
<xml_diff>
--- a/resources/analysis_of_algorithms.xlsx
+++ b/resources/analysis_of_algorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/murillo/development/project/git/private/estudos/searching-sorting-algorithms/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2819C2E-9947-204C-B89C-C043E64D2313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A600B9DF-66F2-C146-A179-3EB5A1D3D3FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="460" windowWidth="37700" windowHeight="21140" activeTab="2" xr2:uid="{947E0903-3BAA-4B47-9B05-889BB2447F05}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>Element Number</t>
   </si>
@@ -117,9 +117,6 @@
     <t>MergeSort and QuickSort</t>
   </si>
   <si>
-    <t>n*O (log₂ n)</t>
-  </si>
-  <si>
     <t>log₂ n</t>
   </si>
   <si>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t>Logarithm</t>
+  </si>
+  <si>
+    <t>n*(log₂ n)</t>
+  </si>
+  <si>
+    <t>O (log₂ n)</t>
   </si>
 </sst>
 </file>
@@ -288,14 +291,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,7 +836,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n*O (log₂ n)</c:v>
+                  <c:v>n*(log₂ n)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5883,7 +5886,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n*O (log₂ n)</c:v>
+                  <c:v>n*(log₂ n)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6030,7 +6033,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n*O (log₂ n)</c:v>
+                  <c:v>n*(log₂ n)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11026,15 +11029,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>108142</xdr:colOff>
+      <xdr:colOff>134878</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>244784</xdr:rowOff>
+      <xdr:rowOff>251469</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>487948</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>187156</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>300789</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11234,15 +11237,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>128193</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>251470</xdr:rowOff>
+      <xdr:colOff>121510</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4155</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>193842</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>521370</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11572,7 +11575,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11587,15 +11590,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -11615,7 +11618,7 @@
         <v>21</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -11635,7 +11638,7 @@
         <v>24</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -11649,16 +11652,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -11735,7 +11738,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" ref="E8:G19" si="4">POWER(A8,3)</f>
+        <f t="shared" ref="E8:E19" si="4">POWER(A8,3)</f>
         <v>64</v>
       </c>
       <c r="F8" s="8">
@@ -11800,7 +11803,7 @@
         <f t="shared" si="2"/>
         <v>65536</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="12">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
@@ -11829,7 +11832,7 @@
         <f t="shared" si="2"/>
         <v>4294967296</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="12">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
@@ -11858,7 +11861,7 @@
         <f t="shared" si="2"/>
         <v>1.8446744073709552E+19</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="12">
         <f t="shared" si="3"/>
         <v>384</v>
       </c>
@@ -11887,7 +11890,7 @@
         <f t="shared" si="2"/>
         <v>3.4028236692093846E+38</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="12">
         <f t="shared" si="3"/>
         <v>896</v>
       </c>
@@ -11916,7 +11919,7 @@
         <f t="shared" si="2"/>
         <v>1.157920892373162E+77</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="12">
         <f t="shared" si="3"/>
         <v>2048</v>
       </c>
@@ -11945,7 +11948,7 @@
         <f t="shared" si="2"/>
         <v>1.3407807929942597E+154</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="12">
         <f t="shared" si="3"/>
         <v>4608</v>
       </c>
@@ -11974,7 +11977,7 @@
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="12">
         <f t="shared" si="3"/>
         <v>10240</v>
       </c>
@@ -12003,7 +12006,7 @@
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="12">
         <f t="shared" si="3"/>
         <v>22528</v>
       </c>
@@ -12032,7 +12035,7 @@
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="12">
         <f t="shared" si="3"/>
         <v>49152</v>
       </c>
@@ -12061,7 +12064,7 @@
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="12">
         <f t="shared" si="3"/>
         <v>106496</v>
       </c>
@@ -12091,15 +12094,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -12329,7 +12332,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12340,15 +12343,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -12362,7 +12365,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -12581,15 +12584,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -12608,10 +12611,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -12834,15 +12837,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -12861,10 +12864,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -13089,15 +13092,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -13122,16 +13125,16 @@
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -13554,10 +13557,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="13"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -13577,10 +13580,10 @@
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -13770,7 +13773,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13780,15 +13783,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -13807,10 +13810,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>